<commit_message>
updating in-model documentation and write up
</commit_message>
<xml_diff>
--- a/background/Supplemental_Excel.xlsx
+++ b/background/Supplemental_Excel.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\OneDrive\Desktop\ReposGoHere\PublicRepos\Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\OneDrive\Desktop\ReposGoHere\PublicRepos\Capstone\background\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="418" documentId="8_{5C73338D-B8EC-4B18-9CAD-7B9B9CA15394}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{1A198F8C-C0AC-45B0-A574-813678FC735F}"/>
+  <xr:revisionPtr revIDLastSave="455" documentId="8_{5C73338D-B8EC-4B18-9CAD-7B9B9CA15394}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{9A4A3EE5-9A97-4F0E-AA1A-3A902E352D63}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4080" activeTab="2" xr2:uid="{261272EC-EE60-44CA-9508-88C02FE8EAF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Engagment Analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="Workflow Map" sheetId="2" r:id="rId2"/>
-    <sheet name="Folder Organization" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
+    <sheet name="Workflow Map" sheetId="2" r:id="rId4"/>
+    <sheet name="Folder Organization" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
   <si>
     <t>Views</t>
   </si>
@@ -92,6 +94,192 @@
   </si>
   <si>
     <t>log Likes / log views</t>
+  </si>
+  <si>
+    <t>Log Ratio</t>
+  </si>
+  <si>
+    <t>B tone - LEAVE STORY Official Video1</t>
+  </si>
+  <si>
+    <t>WHY HOLD BACK - Trunk Boiz member B*Janky</t>
+  </si>
+  <si>
+    <t>Jonathan C. Meier - Savage (Audio)</t>
+  </si>
+  <si>
+    <t>HeartLand Didgeridoo - key of C - (4701)</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Genomineerden gouden C 2017</t>
+  </si>
+  <si>
+    <t>DELAIN /SING TO ME /c/ MARCO HIETALA 6/ en MAL...</t>
+  </si>
+  <si>
+    <t>Tram,Bix and Lang - For no reason at all in C ...</t>
+  </si>
+  <si>
+    <t>Catalogue d'Emojis Teaser</t>
+  </si>
+  <si>
+    <t>view_class</t>
+  </si>
+  <si>
+    <t>caption</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>licensedContent</t>
+  </si>
+  <si>
+    <t>regionRestriction</t>
+  </si>
+  <si>
+    <t>contentRating</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>month_day</t>
+  </si>
+  <si>
+    <t>year_day</t>
+  </si>
+  <si>
+    <t>week_day</t>
+  </si>
+  <si>
+    <t>week</t>
+  </si>
+  <si>
+    <t>description_sentiment</t>
+  </si>
+  <si>
+    <t>description_wordcount</t>
+  </si>
+  <si>
+    <t>tags_sentiment</t>
+  </si>
+  <si>
+    <t>tags_wordcount</t>
+  </si>
+  <si>
+    <t>title_sentiment</t>
+  </si>
+  <si>
+    <t>title_wordcount</t>
+  </si>
+  <si>
+    <t>title_featuring</t>
+  </si>
+  <si>
+    <t>intitle_a</t>
+  </si>
+  <si>
+    <t>intitle_b</t>
+  </si>
+  <si>
+    <t>intitle_c</t>
+  </si>
+  <si>
+    <t>intitle_d</t>
+  </si>
+  <si>
+    <t>intitle_e</t>
+  </si>
+  <si>
+    <t>intitle_f</t>
+  </si>
+  <si>
+    <t>intitle_g</t>
+  </si>
+  <si>
+    <t>intitle_h</t>
+  </si>
+  <si>
+    <t>intitle_i</t>
+  </si>
+  <si>
+    <t>intitle_j</t>
+  </si>
+  <si>
+    <t>intitle_k</t>
+  </si>
+  <si>
+    <t>intitle_l</t>
+  </si>
+  <si>
+    <t>intitle_m</t>
+  </si>
+  <si>
+    <t>intitle_n</t>
+  </si>
+  <si>
+    <t>intitle_o</t>
+  </si>
+  <si>
+    <t>intitle_p</t>
+  </si>
+  <si>
+    <t>intitle_q</t>
+  </si>
+  <si>
+    <t>intitle_r</t>
+  </si>
+  <si>
+    <t>intitle_s</t>
+  </si>
+  <si>
+    <t>intitle_t</t>
+  </si>
+  <si>
+    <t>intitle_u</t>
+  </si>
+  <si>
+    <t>intitle_v</t>
+  </si>
+  <si>
+    <t>intitle_w</t>
+  </si>
+  <si>
+    <t>intitle_x</t>
+  </si>
+  <si>
+    <t>intitle_y</t>
+  </si>
+  <si>
+    <t>intitle_z</t>
+  </si>
+  <si>
+    <t>title_length</t>
+  </si>
+  <si>
+    <t>lv_ratio</t>
+  </si>
+  <si>
+    <t>comment_view_ratio</t>
+  </si>
+  <si>
+    <t>like_dislike_ratio</t>
+  </si>
+  <si>
+    <t>is_weekend</t>
+  </si>
+  <si>
+    <t>is_friday</t>
   </si>
 </sst>
 </file>
@@ -317,7 +505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -407,6 +595,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12670,7 +12867,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93511403-65C8-42C9-8D10-FBFAE41D1123}">
   <dimension ref="B2:P20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:K14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -12694,7 +12893,9 @@
       <c r="E2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="H2" s="9" t="s">
         <v>0</v>
       </c>
@@ -13004,6 +13205,1935 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AF41F9-E12C-41D8-BD07-B453BFE1B6E6}">
+  <dimension ref="B1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="42.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B2" s="16">
+        <v>240</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B3" s="16">
+        <v>159</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B4" s="16">
+        <v>112</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B5" s="16">
+        <v>58</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B6" s="15">
+        <v>157</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B7" s="15">
+        <v>26</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B8" s="15">
+        <v>87</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B9" s="15">
+        <v>270</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00300CDE-6568-4DFC-B14F-0FAD2A8F72D8}">
+  <dimension ref="B2:L53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="9.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="37">
+        <v>0</v>
+      </c>
+      <c r="D2" s="37">
+        <v>1</v>
+      </c>
+      <c r="E2" s="37">
+        <v>2</v>
+      </c>
+      <c r="F2" s="37">
+        <v>3</v>
+      </c>
+      <c r="G2" s="37">
+        <v>4</v>
+      </c>
+      <c r="H2" s="37">
+        <v>5</v>
+      </c>
+      <c r="I2" s="37">
+        <v>6</v>
+      </c>
+      <c r="J2" s="37">
+        <v>7</v>
+      </c>
+      <c r="K2" s="37">
+        <v>8</v>
+      </c>
+      <c r="L2" s="37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.4493000000000001E-2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1.1254E-2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2.3255999999999999E-2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>5.0146999999999997E-2</v>
+      </c>
+      <c r="I3" s="2">
+        <v>5.9885000000000001E-2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.107143</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.20613500000000001</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.76190500000000005</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.84506999999999999</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.81642499999999996</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.72829600000000005</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.68459300000000001</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.65265499999999999</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.65340399999999998</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.69322300000000003</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.802454</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.96470599999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="39">
+        <v>701.28571399999998</v>
+      </c>
+      <c r="D5" s="39">
+        <v>416.56338</v>
+      </c>
+      <c r="E5" s="39">
+        <v>500.16425099999998</v>
+      </c>
+      <c r="F5" s="39">
+        <v>519.47427700000003</v>
+      </c>
+      <c r="G5" s="39">
+        <v>753.05959299999995</v>
+      </c>
+      <c r="H5" s="39">
+        <v>778.47418900000002</v>
+      </c>
+      <c r="I5" s="39">
+        <v>631.09598000000005</v>
+      </c>
+      <c r="J5" s="39">
+        <v>336.24358999999998</v>
+      </c>
+      <c r="K5" s="39">
+        <v>256.54601200000002</v>
+      </c>
+      <c r="L5" s="39">
+        <v>256.17647099999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.85714299999999999</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.29577500000000001</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.27053100000000002</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.36816700000000002</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.44476700000000002</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.47713899999999998</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.55168200000000001</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.711538</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.88466299999999998</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.98823499999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.61904800000000004</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2.8169E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>9.6460000000000001E-3</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4.2151000000000001E-2</v>
+      </c>
+      <c r="H7" s="2">
+        <v>7.3746000000000006E-2</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.12510299999999999</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.19139200000000001</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.26625799999999999</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.30588199999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.6080000000000001E-3</v>
+      </c>
+      <c r="G8" s="2">
+        <v>4.3600000000000002E-3</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1.475E-3</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1.2310000000000001E-3</v>
+      </c>
+      <c r="J8" s="2">
+        <v>3.663E-3</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="2">
+        <v>17.761904999999999</v>
+      </c>
+      <c r="D9" s="2">
+        <v>17.661971999999999</v>
+      </c>
+      <c r="E9" s="2">
+        <v>16.782609000000001</v>
+      </c>
+      <c r="F9" s="2">
+        <v>14.818327999999999</v>
+      </c>
+      <c r="G9" s="2">
+        <v>14.537791</v>
+      </c>
+      <c r="H9" s="2">
+        <v>14.207965</v>
+      </c>
+      <c r="I9" s="2">
+        <v>13.853158000000001</v>
+      </c>
+      <c r="J9" s="2">
+        <v>13.732601000000001</v>
+      </c>
+      <c r="K9" s="2">
+        <v>14.09816</v>
+      </c>
+      <c r="L9" s="2">
+        <v>14.282353000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="2">
+        <v>8.6666670000000003</v>
+      </c>
+      <c r="D10" s="2">
+        <v>7.901408</v>
+      </c>
+      <c r="E10" s="2">
+        <v>7.0579710000000002</v>
+      </c>
+      <c r="F10" s="2">
+        <v>7.1881029999999999</v>
+      </c>
+      <c r="G10" s="2">
+        <v>7.0276160000000001</v>
+      </c>
+      <c r="H10" s="2">
+        <v>6.898968</v>
+      </c>
+      <c r="I10" s="2">
+        <v>6.7391300000000003</v>
+      </c>
+      <c r="J10" s="2">
+        <v>6.6543039999999998</v>
+      </c>
+      <c r="K10" s="2">
+        <v>6.8527610000000001</v>
+      </c>
+      <c r="L10" s="2">
+        <v>6.364706</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2">
+        <v>24.190476</v>
+      </c>
+      <c r="D11" s="2">
+        <v>12.126761</v>
+      </c>
+      <c r="E11" s="2">
+        <v>17.161836000000001</v>
+      </c>
+      <c r="F11" s="2">
+        <v>17.287780999999999</v>
+      </c>
+      <c r="G11" s="2">
+        <v>17.931685999999999</v>
+      </c>
+      <c r="H11" s="2">
+        <v>16.797198000000002</v>
+      </c>
+      <c r="I11" s="2">
+        <v>16.312550999999999</v>
+      </c>
+      <c r="J11" s="2">
+        <v>16.190476</v>
+      </c>
+      <c r="K11" s="2">
+        <v>15.802454000000001</v>
+      </c>
+      <c r="L11" s="2">
+        <v>16.847059000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="39">
+        <v>256.85714300000001</v>
+      </c>
+      <c r="D12" s="39">
+        <v>221.267606</v>
+      </c>
+      <c r="E12" s="39">
+        <v>200.741546</v>
+      </c>
+      <c r="F12" s="39">
+        <v>204.94051400000001</v>
+      </c>
+      <c r="G12" s="39">
+        <v>200.688953</v>
+      </c>
+      <c r="H12" s="39">
+        <v>195.64085499999999</v>
+      </c>
+      <c r="I12" s="39">
+        <v>190.26250999999999</v>
+      </c>
+      <c r="J12" s="39">
+        <v>187.519689</v>
+      </c>
+      <c r="K12" s="39">
+        <v>193.16932499999999</v>
+      </c>
+      <c r="L12" s="39">
+        <v>179.34117599999999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4.5714290000000002</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2.1690140000000002</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2.9178739999999999</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3.041801</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2.9098839999999999</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2.9203540000000001</v>
+      </c>
+      <c r="I13" s="2">
+        <v>2.8712059999999999</v>
+      </c>
+      <c r="J13" s="2">
+        <v>2.8722530000000002</v>
+      </c>
+      <c r="K13" s="2">
+        <v>2.8294480000000002</v>
+      </c>
+      <c r="L13" s="2">
+        <v>2.5764710000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="2">
+        <v>36.904761999999998</v>
+      </c>
+      <c r="D14" s="2">
+        <v>32.126761000000002</v>
+      </c>
+      <c r="E14" s="2">
+        <v>29.067633000000001</v>
+      </c>
+      <c r="F14" s="2">
+        <v>29.570740000000001</v>
+      </c>
+      <c r="G14" s="2">
+        <v>29.023256</v>
+      </c>
+      <c r="H14" s="2">
+        <v>28.341445</v>
+      </c>
+      <c r="I14" s="2">
+        <v>27.699344</v>
+      </c>
+      <c r="J14" s="2">
+        <v>27.180402999999998</v>
+      </c>
+      <c r="K14" s="2">
+        <v>28.012270000000001</v>
+      </c>
+      <c r="L14" s="2">
+        <v>26.082353000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-1.0219999999999999E-3</v>
+      </c>
+      <c r="D15" s="2">
+        <v>4.5832999999999999E-2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>8.3450999999999997E-2</v>
+      </c>
+      <c r="F15" s="2">
+        <v>9.2135999999999996E-2</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.109011</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.116163</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.133491</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.15559600000000001</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.15146899999999999</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.19031699999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="2">
+        <v>35.142856999999999</v>
+      </c>
+      <c r="D16" s="2">
+        <v>47.859155000000001</v>
+      </c>
+      <c r="E16" s="2">
+        <v>50.007246000000002</v>
+      </c>
+      <c r="F16" s="2">
+        <v>65.085209000000006</v>
+      </c>
+      <c r="G16" s="2">
+        <v>76.495639999999995</v>
+      </c>
+      <c r="H16" s="2">
+        <v>81.329645999999997</v>
+      </c>
+      <c r="I16" s="2">
+        <v>90.515586999999996</v>
+      </c>
+      <c r="J16" s="2">
+        <v>111.707418</v>
+      </c>
+      <c r="K16" s="2">
+        <v>121.468712</v>
+      </c>
+      <c r="L16" s="2">
+        <v>128.31764699999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="2">
+        <v>9.9989999999999992E-3</v>
+      </c>
+      <c r="D17" s="2">
+        <v>8.2719999999999998E-3</v>
+      </c>
+      <c r="E17" s="2">
+        <v>4.7810999999999999E-2</v>
+      </c>
+      <c r="F17" s="2">
+        <v>3.2458000000000001E-2</v>
+      </c>
+      <c r="G17" s="2">
+        <v>2.6067E-2</v>
+      </c>
+      <c r="H17" s="2">
+        <v>5.1778999999999999E-2</v>
+      </c>
+      <c r="I17" s="2">
+        <v>6.4217999999999997E-2</v>
+      </c>
+      <c r="J17" s="2">
+        <v>7.6594999999999996E-2</v>
+      </c>
+      <c r="K17" s="2">
+        <v>5.1457999999999997E-2</v>
+      </c>
+      <c r="L17" s="2">
+        <v>6.028E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="2">
+        <v>6.6190480000000003</v>
+      </c>
+      <c r="D18" s="2">
+        <v>8.2253520000000009</v>
+      </c>
+      <c r="E18" s="2">
+        <v>9.0748789999999993</v>
+      </c>
+      <c r="F18" s="2">
+        <v>10.546624</v>
+      </c>
+      <c r="G18" s="2">
+        <v>12.359012</v>
+      </c>
+      <c r="H18" s="2">
+        <v>12.257375</v>
+      </c>
+      <c r="I18" s="2">
+        <v>14.160788</v>
+      </c>
+      <c r="J18" s="2">
+        <v>16.682234000000001</v>
+      </c>
+      <c r="K18" s="2">
+        <v>17.78773</v>
+      </c>
+      <c r="L18" s="2">
+        <v>17.776471000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="2">
+        <v>-3.9418000000000002E-2</v>
+      </c>
+      <c r="D19" s="2">
+        <v>-1.792E-3</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.8475999999999999E-2</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1.9907000000000001E-2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>2.4681999999999999E-2</v>
+      </c>
+      <c r="H19" s="2">
+        <v>3.6450000000000003E-2</v>
+      </c>
+      <c r="I19" s="2">
+        <v>4.6116999999999998E-2</v>
+      </c>
+      <c r="J19" s="2">
+        <v>3.9941999999999998E-2</v>
+      </c>
+      <c r="K19" s="2">
+        <v>2.6533000000000001E-2</v>
+      </c>
+      <c r="L19" s="2">
+        <v>9.3329999999999993E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="2">
+        <v>4.6666670000000003</v>
+      </c>
+      <c r="D20" s="2">
+        <v>6.901408</v>
+      </c>
+      <c r="E20" s="2">
+        <v>6.7632849999999998</v>
+      </c>
+      <c r="F20" s="2">
+        <v>7.5160770000000001</v>
+      </c>
+      <c r="G20" s="2">
+        <v>8.2238369999999996</v>
+      </c>
+      <c r="H20" s="2">
+        <v>7.9837759999999998</v>
+      </c>
+      <c r="I20" s="2">
+        <v>7.848236</v>
+      </c>
+      <c r="J20" s="2">
+        <v>8.0352560000000004</v>
+      </c>
+      <c r="K20" s="2">
+        <v>7.5865030000000004</v>
+      </c>
+      <c r="L20" s="2">
+        <v>7.2352939999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="2">
+        <v>4.7619000000000002E-2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>3.8647000000000001E-2</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5.4662000000000002E-2</v>
+      </c>
+      <c r="G21" s="2">
+        <v>7.1221000000000007E-2</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.105457</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.12674299999999999</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0.18727099999999999</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0.26993899999999998</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0.376471</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1.714286</v>
+      </c>
+      <c r="D22" s="2">
+        <v>2.0422539999999998</v>
+      </c>
+      <c r="E22" s="2">
+        <v>2.4057970000000002</v>
+      </c>
+      <c r="F22" s="2">
+        <v>2.5739550000000002</v>
+      </c>
+      <c r="G22" s="2">
+        <v>2.6031979999999999</v>
+      </c>
+      <c r="H22" s="2">
+        <v>2.5914450000000002</v>
+      </c>
+      <c r="I22" s="2">
+        <v>2.611977</v>
+      </c>
+      <c r="J22" s="2">
+        <v>2.7316850000000001</v>
+      </c>
+      <c r="K22" s="2">
+        <v>2.8613499999999998</v>
+      </c>
+      <c r="L22" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.28571400000000002</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.29577500000000001</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.26086999999999999</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.27652700000000002</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.31976700000000002</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.26843699999999998</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0.25799800000000001</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.23488999999999999</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0.16441700000000001</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0.17647099999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.28571400000000002</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.70422499999999999</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.74154600000000004</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.77492000000000005</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.76744199999999996</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.89306799999999997</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0.92616900000000002</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0.90613600000000005</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0.84171799999999997</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0.88235300000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.33333299999999999</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.84506999999999999</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.76570000000000005</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.82958200000000004</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.92296500000000004</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.79719799999999996</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0.87653800000000004</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0.94276599999999999</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0.93006100000000003</v>
+      </c>
+      <c r="L25" s="2">
+        <v>1.0705880000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1.9047620000000001</v>
+      </c>
+      <c r="D26" s="2">
+        <v>2.1549299999999998</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2.6835749999999998</v>
+      </c>
+      <c r="F26" s="2">
+        <v>2.7765270000000002</v>
+      </c>
+      <c r="G26" s="2">
+        <v>2.7572670000000001</v>
+      </c>
+      <c r="H26" s="2">
+        <v>2.8650440000000001</v>
+      </c>
+      <c r="I26" s="2">
+        <v>2.851928</v>
+      </c>
+      <c r="J26" s="2">
+        <v>2.8997250000000001</v>
+      </c>
+      <c r="K26" s="2">
+        <v>2.9092020000000001</v>
+      </c>
+      <c r="L26" s="2">
+        <v>2.9058820000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.19047600000000001</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.15493000000000001</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.28743999999999997</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.32315100000000002</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.42296499999999998</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0.48008800000000001</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0.58818700000000002</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0.730769</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0.95214699999999997</v>
+      </c>
+      <c r="L27" s="2">
+        <v>1.329412</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.42857099999999998</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.338028</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.44202900000000001</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.42925999999999997</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.453488</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0.41814200000000001</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0.39868700000000001</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0.40201500000000001</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0.360736</v>
+      </c>
+      <c r="L28" s="2">
+        <v>0.28235300000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.42857099999999998</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.64788699999999999</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.65217400000000003</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.74758800000000003</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.765988</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.79351000000000005</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0.66858099999999998</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0.67490799999999995</v>
+      </c>
+      <c r="K29" s="2">
+        <v>0.73128800000000005</v>
+      </c>
+      <c r="L29" s="2">
+        <v>0.78823500000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1.0952379999999999</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1.6338029999999999</v>
+      </c>
+      <c r="E30" s="2">
+        <v>2.1328499999999999</v>
+      </c>
+      <c r="F30" s="2">
+        <v>2.1045020000000001</v>
+      </c>
+      <c r="G30" s="2">
+        <v>2.3648259999999999</v>
+      </c>
+      <c r="H30" s="2">
+        <v>2.5398230000000002</v>
+      </c>
+      <c r="I30" s="2">
+        <v>2.5131260000000002</v>
+      </c>
+      <c r="J30" s="2">
+        <v>2.7564099999999998</v>
+      </c>
+      <c r="K30" s="2">
+        <v>2.8625769999999999</v>
+      </c>
+      <c r="L30" s="2">
+        <v>2.9764710000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <v>8.4506999999999999E-2</v>
+      </c>
+      <c r="E31" s="2">
+        <v>9.6617999999999996E-2</v>
+      </c>
+      <c r="F31" s="2">
+        <v>9.8071000000000005E-2</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.107558</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0.102507</v>
+      </c>
+      <c r="I31" s="2">
+        <v>7.5062000000000004E-2</v>
+      </c>
+      <c r="J31" s="2">
+        <v>8.4707000000000005E-2</v>
+      </c>
+      <c r="K31" s="2">
+        <v>6.6257999999999997E-2</v>
+      </c>
+      <c r="L31" s="2">
+        <v>4.7058999999999997E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.19047600000000001</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.32394400000000001</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.33574900000000002</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.30707400000000001</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.33284900000000001</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0.35324499999999998</v>
+      </c>
+      <c r="I32" s="2">
+        <v>0.31173099999999998</v>
+      </c>
+      <c r="J32" s="2">
+        <v>0.32509199999999999</v>
+      </c>
+      <c r="K32" s="2">
+        <v>0.35214699999999999</v>
+      </c>
+      <c r="L32" s="2">
+        <v>0.47058800000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.80952400000000002</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1.0704229999999999</v>
+      </c>
+      <c r="E33" s="2">
+        <v>1.3188409999999999</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1.310289</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1.318314</v>
+      </c>
+      <c r="H33" s="2">
+        <v>1.4587019999999999</v>
+      </c>
+      <c r="I33" s="2">
+        <v>1.4688270000000001</v>
+      </c>
+      <c r="J33" s="2">
+        <v>1.5366299999999999</v>
+      </c>
+      <c r="K33" s="2">
+        <v>1.504294</v>
+      </c>
+      <c r="L33" s="2">
+        <v>1.576471</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.14285700000000001</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.49295800000000001</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0.64009700000000003</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0.69774899999999995</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0.68023299999999998</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0.69469000000000003</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0.62838400000000005</v>
+      </c>
+      <c r="J34" s="2">
+        <v>0.60302199999999995</v>
+      </c>
+      <c r="K34" s="2">
+        <v>0.54233100000000001</v>
+      </c>
+      <c r="L34" s="2">
+        <v>0.611765</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1.142857</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1.323944</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1.8140099999999999</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1.810289</v>
+      </c>
+      <c r="G35" s="2">
+        <v>2.0334300000000001</v>
+      </c>
+      <c r="H35" s="2">
+        <v>2.0221239999999998</v>
+      </c>
+      <c r="I35" s="2">
+        <v>1.8207549999999999</v>
+      </c>
+      <c r="J35" s="2">
+        <v>1.746337</v>
+      </c>
+      <c r="K35" s="2">
+        <v>1.75092</v>
+      </c>
+      <c r="L35" s="2">
+        <v>1.7176469999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="2">
+        <v>1.7619050000000001</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1.9295770000000001</v>
+      </c>
+      <c r="E36" s="2">
+        <v>1.8623190000000001</v>
+      </c>
+      <c r="F36" s="2">
+        <v>2.0819939999999999</v>
+      </c>
+      <c r="G36" s="2">
+        <v>2.318314</v>
+      </c>
+      <c r="H36" s="2">
+        <v>2.3266960000000001</v>
+      </c>
+      <c r="I36" s="2">
+        <v>2.2932730000000001</v>
+      </c>
+      <c r="J36" s="2">
+        <v>2.261447</v>
+      </c>
+      <c r="K36" s="2">
+        <v>2.136196</v>
+      </c>
+      <c r="L36" s="2">
+        <v>2.011765</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.47619</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.43662000000000001</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.38164300000000001</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.46784599999999998</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0.48837199999999997</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0.47640100000000002</v>
+      </c>
+      <c r="I37" s="2">
+        <v>0.37735800000000003</v>
+      </c>
+      <c r="J37" s="2">
+        <v>0.34340700000000002</v>
+      </c>
+      <c r="K37" s="2">
+        <v>0.27607399999999999</v>
+      </c>
+      <c r="L37" s="2">
+        <v>0.28235300000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0</v>
+      </c>
+      <c r="D38" s="2">
+        <v>7.0422999999999999E-2</v>
+      </c>
+      <c r="E38" s="2">
+        <v>4.5893999999999997E-2</v>
+      </c>
+      <c r="F38" s="2">
+        <v>4.0193E-2</v>
+      </c>
+      <c r="G38" s="2">
+        <v>3.1976999999999998E-2</v>
+      </c>
+      <c r="H38" s="2">
+        <v>3.6873000000000003E-2</v>
+      </c>
+      <c r="I38" s="2">
+        <v>3.6095000000000002E-2</v>
+      </c>
+      <c r="J38" s="2">
+        <v>3.6630000000000003E-2</v>
+      </c>
+      <c r="K38" s="2">
+        <v>3.3128999999999999E-2</v>
+      </c>
+      <c r="L38" s="2">
+        <v>3.5293999999999999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1.2380949999999999</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1.56338</v>
+      </c>
+      <c r="E39" s="2">
+        <v>1.562802</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1.6816720000000001</v>
+      </c>
+      <c r="G39" s="2">
+        <v>1.8648260000000001</v>
+      </c>
+      <c r="H39" s="2">
+        <v>1.778761</v>
+      </c>
+      <c r="I39" s="2">
+        <v>1.586136</v>
+      </c>
+      <c r="J39" s="2">
+        <v>1.5325089999999999</v>
+      </c>
+      <c r="K39" s="2">
+        <v>1.370552</v>
+      </c>
+      <c r="L39" s="2">
+        <v>1.4941180000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.66666700000000001</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1.0704229999999999</v>
+      </c>
+      <c r="E40" s="2">
+        <v>1.4227050000000001</v>
+      </c>
+      <c r="F40" s="2">
+        <v>1.263666</v>
+      </c>
+      <c r="G40" s="2">
+        <v>1.199128</v>
+      </c>
+      <c r="H40" s="2">
+        <v>1.2330380000000001</v>
+      </c>
+      <c r="I40" s="2">
+        <v>1.223544</v>
+      </c>
+      <c r="J40" s="2">
+        <v>1.160256</v>
+      </c>
+      <c r="K40" s="2">
+        <v>1.06135</v>
+      </c>
+      <c r="L40" s="2">
+        <v>0.90588199999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.95238100000000003</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1.169014</v>
+      </c>
+      <c r="E41" s="2">
+        <v>1.323671</v>
+      </c>
+      <c r="F41" s="2">
+        <v>1.448553</v>
+      </c>
+      <c r="G41" s="2">
+        <v>1.4985470000000001</v>
+      </c>
+      <c r="H41" s="2">
+        <v>1.4550149999999999</v>
+      </c>
+      <c r="I41" s="2">
+        <v>1.3191139999999999</v>
+      </c>
+      <c r="J41" s="2">
+        <v>1.2953300000000001</v>
+      </c>
+      <c r="K41" s="2">
+        <v>1.3754599999999999</v>
+      </c>
+      <c r="L41" s="2">
+        <v>1.2823530000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.42857099999999998</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.61971799999999999</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0.91787399999999997</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.86816700000000002</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0.93895300000000004</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0.94174000000000002</v>
+      </c>
+      <c r="I42" s="2">
+        <v>0.90935200000000005</v>
+      </c>
+      <c r="J42" s="2">
+        <v>0.89285700000000001</v>
+      </c>
+      <c r="K42" s="2">
+        <v>0.82944799999999996</v>
+      </c>
+      <c r="L42" s="2">
+        <v>0.96470599999999995</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.238095</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.29577500000000001</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0.28985499999999997</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.31028899999999998</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0.32558100000000001</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0.331121</v>
+      </c>
+      <c r="I43" s="2">
+        <v>0.31665300000000002</v>
+      </c>
+      <c r="J43" s="2">
+        <v>0.283883</v>
+      </c>
+      <c r="K43" s="2">
+        <v>0.30061300000000002</v>
+      </c>
+      <c r="L43" s="2">
+        <v>0.17647099999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.19047600000000001</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.29577500000000001</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0.23913000000000001</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.229904</v>
+      </c>
+      <c r="G44" s="2">
+        <v>0.21366299999999999</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0.17551600000000001</v>
+      </c>
+      <c r="I44" s="2">
+        <v>0.17760500000000001</v>
+      </c>
+      <c r="J44" s="2">
+        <v>0.144231</v>
+      </c>
+      <c r="K44" s="2">
+        <v>0.14233100000000001</v>
+      </c>
+      <c r="L44" s="2">
+        <v>0.15294099999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="2">
+        <v>9.5238000000000003E-2</v>
+      </c>
+      <c r="D45" s="2">
+        <v>5.6337999999999999E-2</v>
+      </c>
+      <c r="E45" s="2">
+        <v>0.12318800000000001</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0.115756</v>
+      </c>
+      <c r="G45" s="2">
+        <v>0.164244</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0.163717</v>
+      </c>
+      <c r="I45" s="2">
+        <v>0.13535700000000001</v>
+      </c>
+      <c r="J45" s="2">
+        <v>0.12912100000000001</v>
+      </c>
+      <c r="K45" s="2">
+        <v>0.13619600000000001</v>
+      </c>
+      <c r="L45" s="2">
+        <v>7.0587999999999998E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.52381</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.50704199999999999</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0.40338200000000002</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0.50160800000000005</v>
+      </c>
+      <c r="G46" s="2">
+        <v>0.56976700000000002</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0.58702100000000002</v>
+      </c>
+      <c r="I46" s="2">
+        <v>0.59516000000000002</v>
+      </c>
+      <c r="J46" s="2">
+        <v>0.664377</v>
+      </c>
+      <c r="K46" s="2">
+        <v>0.54601200000000005</v>
+      </c>
+      <c r="L46" s="2">
+        <v>0.65882399999999997</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>75</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.14285700000000001</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.26760600000000001</v>
+      </c>
+      <c r="E47" s="2">
+        <v>0.25362299999999999</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0.200965</v>
+      </c>
+      <c r="G47" s="2">
+        <v>0.21802299999999999</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0.17846600000000001</v>
+      </c>
+      <c r="I47" s="2">
+        <v>0.15340400000000001</v>
+      </c>
+      <c r="J47" s="2">
+        <v>0.156136</v>
+      </c>
+      <c r="K47" s="2">
+        <v>0.112883</v>
+      </c>
+      <c r="L47" s="2">
+        <v>0.15294099999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48" s="2">
+        <v>27.619047999999999</v>
+      </c>
+      <c r="D48" s="2">
+        <v>39.380282000000001</v>
+      </c>
+      <c r="E48" s="2">
+        <v>42.818840999999999</v>
+      </c>
+      <c r="F48" s="2">
+        <v>46.012861999999998</v>
+      </c>
+      <c r="G48" s="2">
+        <v>49.704942000000003</v>
+      </c>
+      <c r="H48" s="2">
+        <v>48.656342000000002</v>
+      </c>
+      <c r="I48" s="2">
+        <v>47.378179000000003</v>
+      </c>
+      <c r="J48" s="2">
+        <v>47.553570999999998</v>
+      </c>
+      <c r="K48" s="2">
+        <v>45.363190000000003</v>
+      </c>
+      <c r="L48" s="2">
+        <v>44.988235000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1.0150220000000001</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.245144</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0.34751399999999999</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0.44345400000000001</v>
+      </c>
+      <c r="G49" s="2">
+        <v>0.55384100000000003</v>
+      </c>
+      <c r="H49" s="2">
+        <v>0.62205100000000002</v>
+      </c>
+      <c r="I49" s="2">
+        <v>0.66504799999999997</v>
+      </c>
+      <c r="J49" s="2">
+        <v>0.69689800000000002</v>
+      </c>
+      <c r="K49" s="2">
+        <v>0.72543999999999997</v>
+      </c>
+      <c r="L49" s="2">
+        <v>0.73762399999999995</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1</v>
+      </c>
+      <c r="D50" s="2">
+        <v>7.7744999999999995E-2</v>
+      </c>
+      <c r="E50" s="2">
+        <v>0.10194599999999999</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0.18004400000000001</v>
+      </c>
+      <c r="G50" s="2">
+        <v>0.32337100000000002</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0.41330099999999997</v>
+      </c>
+      <c r="I50" s="2">
+        <v>0.46317799999999998</v>
+      </c>
+      <c r="J50" s="2">
+        <v>0.51217599999999996</v>
+      </c>
+      <c r="K50" s="2">
+        <v>0.568272</v>
+      </c>
+      <c r="L50" s="2">
+        <v>0.59927399999999997</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>79</v>
+      </c>
+      <c r="C51" s="2">
+        <v>1.5150170000000001</v>
+      </c>
+      <c r="D51" s="2">
+        <v>6.5774650000000001</v>
+      </c>
+      <c r="E51" s="2">
+        <v>8.2165320000000008</v>
+      </c>
+      <c r="F51" s="2">
+        <v>7.2605079999999997</v>
+      </c>
+      <c r="G51" s="2">
+        <v>3.482399</v>
+      </c>
+      <c r="H51" s="2">
+        <v>1.8378319999999999</v>
+      </c>
+      <c r="I51" s="2">
+        <v>1.497908</v>
+      </c>
+      <c r="J51" s="2">
+        <v>1.3631580000000001</v>
+      </c>
+      <c r="K51" s="2">
+        <v>1.27664</v>
+      </c>
+      <c r="L51" s="2">
+        <v>1.2152160000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.71428599999999998</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0.169014</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0.27053100000000002</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0.28295799999999999</v>
+      </c>
+      <c r="G52" s="2">
+        <v>0.222384</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0.210177</v>
+      </c>
+      <c r="I52" s="2">
+        <v>0.2137</v>
+      </c>
+      <c r="J52" s="2">
+        <v>0.19459699999999999</v>
+      </c>
+      <c r="K52" s="2">
+        <v>0.15828200000000001</v>
+      </c>
+      <c r="L52" s="2">
+        <v>5.8824000000000001E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>81</v>
+      </c>
+      <c r="C53" s="2">
+        <v>9.5238000000000003E-2</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.12676100000000001</v>
+      </c>
+      <c r="E53" s="2">
+        <v>0.154589</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0.17041799999999999</v>
+      </c>
+      <c r="G53" s="2">
+        <v>0.1875</v>
+      </c>
+      <c r="H53" s="2">
+        <v>0.222714</v>
+      </c>
+      <c r="I53" s="2">
+        <v>0.197293</v>
+      </c>
+      <c r="J53" s="2">
+        <v>0.22619</v>
+      </c>
+      <c r="K53" s="2">
+        <v>0.28343600000000002</v>
+      </c>
+      <c r="L53" s="2">
+        <v>0.30588199999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA93D87-C1D9-4C02-9C75-3797DDA0A849}">
   <dimension ref="A1:BO95"/>
   <sheetViews>
@@ -13128,11 +15258,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C5F6F7-DFED-450D-9AF6-86F48E760633}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>

</xml_diff>